<commit_message>
NumberFormat setGroupingUsed(false)  数字转字符串不分组  从  11111111 -> "11,111,111"  修改为 11111111 -> "11111111"
</commit_message>
<xml_diff>
--- a/src/test/resources/test-file/write-template.xlsx
+++ b/src/test/resources/test-file/write-template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>字符串</t>
     <rPh sb="0" eb="1">
@@ -36,13 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>数字</t>
-    <rPh sb="0" eb="1">
-      <t>shu zi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>日期</t>
     <rPh sb="0" eb="1">
       <t>ri qi</t>
@@ -83,6 +76,20 @@
   </si>
   <si>
     <t>MAP B null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字Int</t>
+    <rPh sb="0" eb="1">
+      <t>shu zi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字Long</t>
+    <rPh sb="0" eb="1">
+      <t>shu zi</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -413,50 +420,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>